<commit_message>
update test cases for visa
</commit_message>
<xml_diff>
--- a/Test Cases/Iteration 2/Iteration 2/Iteration 2 Test Cases v2.1 - Result v2.xlsx
+++ b/Test Cases/Iteration 2/Iteration 2/Iteration 2 Test Cases v2.1 - Result v2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1662" yWindow="462" windowWidth="17118" windowHeight="15540" tabRatio="674" firstSheet="4" activeTab="5"/>
+    <workbookView xWindow="1662" yWindow="462" windowWidth="17118" windowHeight="15540" tabRatio="674" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Analysis - Doctor" sheetId="12" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="66">
   <si>
     <t>No</t>
   </si>
@@ -600,6 +600,33 @@
 80 - 90  : 0</t>
     </r>
   </si>
+  <si>
+    <t>team = visa
+start date = 2016 Oct 1
+end date = 2016 Oct 15</t>
+  </si>
+  <si>
+    <t>team = visa
+start date = 2016 Oct 15
+end date = 2016 Oct 31</t>
+  </si>
+  <si>
+    <t>indonesian count = 0 
+non-indonesian count = 0</t>
+  </si>
+  <si>
+    <t>indonesian count = 0 
+non-indonesian count = 2</t>
+  </si>
+  <si>
+    <t>team = visa
+start date = 2016 Nov 1
+end date = 2017 Dec 31</t>
+  </si>
+  <si>
+    <t>indonesian count = 2 
+non-indonesian count = 2</t>
+  </si>
 </sst>
 </file>
 
@@ -692,7 +719,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -723,6 +750,12 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1313,33 +1346,87 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C1" sqref="A1:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
+  <cols>
+    <col min="2" max="2" width="18.34765625" customWidth="1"/>
+    <col min="3" max="3" width="24.84765625" customWidth="1"/>
+    <col min="4" max="4" width="23.296875" customWidth="1"/>
+    <col min="5" max="5" width="13.8984375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.6">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="16" t="s">
         <v>4</v>
       </c>
+    </row>
+    <row r="2" spans="1:6" ht="62.4" x14ac:dyDescent="0.6">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+    </row>
+    <row r="3" spans="1:6" ht="62.4" x14ac:dyDescent="0.6">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+    </row>
+    <row r="4" spans="1:6" ht="62.4" x14ac:dyDescent="0.6">
+      <c r="A4" s="17">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1350,7 +1437,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -1431,7 +1518,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="57" zoomScaleNormal="57" workbookViewId="0">
+    <sheetView zoomScale="57" zoomScaleNormal="57" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update test cases (blank) + result and bug log and metric
</commit_message>
<xml_diff>
--- a/Test Cases/Iteration 2/Iteration 2/Iteration 2 Test Cases v2.1 - Result v2.xlsx
+++ b/Test Cases/Iteration 2/Iteration 2/Iteration 2 Test Cases v2.1 - Result v2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1662" yWindow="462" windowWidth="17118" windowHeight="15540" tabRatio="674" firstSheet="3" activeTab="4"/>
+    <workbookView xWindow="1662" yWindow="462" windowWidth="17118" windowHeight="15540" tabRatio="674" firstSheet="3" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Analysis - Doctor" sheetId="12" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Gender and Age" sheetId="13" r:id="rId6"/>
     <sheet name="Client -  CRUD" sheetId="17" state="hidden" r:id="rId7"/>
     <sheet name="Screening - CRUD " sheetId="18" r:id="rId8"/>
+    <sheet name="Client - CRUD" sheetId="20" r:id="rId9"/>
   </sheets>
   <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="75">
   <si>
     <t>No</t>
   </si>
@@ -72,10 +73,6 @@
     <t>team = medical 
 start date = 2016 Oct 1
 end date = 2016 Oct 15</t>
-  </si>
-  <si>
-    <t>inpatient count = 4 
-outpatient count = 1</t>
   </si>
   <si>
     <t>team = medical 
@@ -304,10 +301,6 @@
   <si>
     <t xml:space="preserve">"Record Added" 
 </t>
-  </si>
-  <si>
-    <t>inpatient count = 3
-outpatient count = 2</t>
   </si>
   <si>
     <t>inpatient count = 0
@@ -390,152 +383,6 @@
   </si>
   <si>
     <t>record deleted</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Female 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0-9 : 0
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>10 - 20 : 1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-20 - 30 : 0
-30 - 40 : 0
-40 - 50 : 0
-50 - 60 : 0
-60 - 70  : 0
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>70 - 80 : 2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-80 - 90  : 0
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Male</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-10 - 20 : 0
-20 - 30 : 0
-30 - 40 : 1  
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>40 - 50 : 1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">z
-50 - 60 : 0
-60 - 70  : 0
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>70 - 80: 7</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-80 - 90  : 0</t>
-    </r>
   </si>
   <si>
     <r>
@@ -611,21 +458,93 @@
 end date = 2016 Oct 31</t>
   </si>
   <si>
-    <t>indonesian count = 0 
-non-indonesian count = 0</t>
-  </si>
-  <si>
-    <t>indonesian count = 0 
-non-indonesian count = 2</t>
-  </si>
-  <si>
     <t>team = visa
 start date = 2016 Nov 1
 end date = 2017 Dec 31</t>
   </si>
   <si>
+    <t xml:space="preserve">Add Client </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Client Name: Tester1 
+Date of Birth: 01/01/1992
+Gender : Female 
+Passport Number :  G123456F
+Client Type: IndividuaNationality : - 
+Referred by: -  
+</t>
+  </si>
+  <si>
+    <t>Success Message shown, client added into the table</t>
+  </si>
+  <si>
+    <t>Edit Client</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Client Name: Tester1 
+Date of Birth: 01/01/1992
+Gender : Female 
+Passport Number :  G123456F
+Client Type: IndividuaNationality : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Indo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Referred by: -  
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Success Message shown, client's nationality edited  added into the table</t>
+  </si>
+  <si>
+    <t>Delete Client</t>
+  </si>
+  <si>
+    <t>Client not shown in table</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Client Shown </t>
+  </si>
+  <si>
+    <t>Changes made not reflected in table and database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Client not shown in table and database </t>
+  </si>
+  <si>
+    <t>inpatient count = 1 
+outpatient count = 0</t>
+  </si>
+  <si>
+    <t>indonesian count = 8 
+non-indonesian count = 14</t>
+  </si>
+  <si>
+    <t>indonesian count = 1 
+non-indonesian count = 1</t>
+  </si>
+  <si>
     <t>indonesian count = 2 
-non-indonesian count = 2</t>
+non-indonesian count = 4</t>
   </si>
 </sst>
 </file>
@@ -749,13 +668,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1081,13 +1000,13 @@
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.6">
@@ -1101,13 +1020,13 @@
         <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="67.8" customHeight="1" x14ac:dyDescent="0.6">
@@ -1121,13 +1040,13 @@
         <v>9</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1180,16 +1099,16 @@
         <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.6">
@@ -1200,16 +1119,16 @@
         <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="46.8" x14ac:dyDescent="0.6">
@@ -1220,16 +1139,16 @@
         <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="F4" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.6">
@@ -1284,19 +1203,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="F2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="46.8" x14ac:dyDescent="0.6">
@@ -1307,16 +1226,16 @@
         <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="E3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="46.8" x14ac:dyDescent="0.6">
@@ -1327,16 +1246,16 @@
         <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="E4" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1348,8 +1267,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:F4"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
@@ -1361,22 +1280,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.6">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="15" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1388,13 +1307,17 @@
         <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
+        <v>74</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="3" spans="1:6" ht="62.4" x14ac:dyDescent="0.6">
       <c r="A3" s="2">
@@ -1404,29 +1327,37 @@
         <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
+        <v>73</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="4" spans="1:6" ht="62.4" x14ac:dyDescent="0.6">
-      <c r="A4" s="17">
+      <c r="A4" s="16">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
+        <v>72</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1437,8 +1368,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView topLeftCell="B1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
@@ -1480,13 +1411,13 @@
         <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="78" x14ac:dyDescent="0.6">
@@ -1497,16 +1428,16 @@
         <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1519,7 +1450,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView zoomScale="57" zoomScaleNormal="57" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
@@ -1560,16 +1491,16 @@
         <v>8</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="F2" s="15" t="s">
-        <v>20</v>
+        <v>56</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.6">
@@ -1643,19 +1574,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="F2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="156" x14ac:dyDescent="0.6">
@@ -1663,19 +1594,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.6">
@@ -1871,8 +1802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="D5" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
@@ -1912,19 +1843,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="F2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -1935,19 +1866,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -1958,19 +1889,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="D4" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G4" s="12"/>
       <c r="H4" s="12"/>
@@ -1981,19 +1912,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="D5" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
@@ -2004,19 +1935,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="F6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
@@ -2027,19 +1958,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
@@ -2115,4 +2046,109 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
+  <cols>
+    <col min="1" max="1" width="3.09765625" customWidth="1"/>
+    <col min="2" max="2" width="12.25" customWidth="1"/>
+    <col min="3" max="3" width="20.546875" customWidth="1"/>
+    <col min="4" max="4" width="15.1484375" customWidth="1"/>
+    <col min="5" max="5" width="12.6484375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.6">
+      <c r="A1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+    </row>
+    <row r="2" spans="1:9" ht="156" x14ac:dyDescent="0.6">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="171.6" x14ac:dyDescent="0.6">
+      <c r="A3" s="16">
+        <v>2</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="171.6" x14ac:dyDescent="0.6">
+      <c r="A4" s="16">
+        <v>3</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>